<commit_message>
Adding OneHotEncode RF model
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422ABA13-8D90-408D-BF30-31B9E81A05C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC42E225-559A-437E-98B1-37E715BC497A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{1F03D750-29BA-4508-AE65-8D8AB8484A6A}"/>
   </bookViews>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAF7CC1-A9BF-42AE-91D3-8A7A36BD33AD}">
   <dimension ref="A1:AD34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated model_rf_65_BiOut_Mix_Breed_Color_BinAge_1Hot NO Mix/Fix
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC42E225-559A-437E-98B1-37E715BC497A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5369E7-FAF4-4427-A5A4-0FF45EEEA407}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{1F03D750-29BA-4508-AE65-8D8AB8484A6A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
   <si>
     <t>Random Forest (Train/Test split)</t>
   </si>
@@ -321,13 +321,193 @@
   </si>
   <si>
     <t>Age categorization is good</t>
+  </si>
+  <si>
+    <t>May 20th</t>
+  </si>
+  <si>
+    <t>model_rf_65_BiOut_Mix_Breed_Color_BinAge_1Hot</t>
+  </si>
+  <si>
+    <t>NO (Top Colors)</t>
+  </si>
+  <si>
+    <t># X features  = 440</t>
+  </si>
+  <si>
+    <t>Fixed_Intact = 0.266037</t>
+  </si>
+  <si>
+    <t>Fixed_Spayed = 0.081024</t>
+  </si>
+  <si>
+    <t>Fixed_Neutered = 0.069082</t>
+  </si>
+  <si>
+    <t>Sex_Male = 0.036651</t>
+  </si>
+  <si>
+    <t>Mix = 0.033081</t>
+  </si>
+  <si>
+    <t>Color2_White = 0.022036</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Baby = 0.014948</t>
+  </si>
+  <si>
+    <t>Color2_Tan = 0.013693</t>
+  </si>
+  <si>
+    <t>Color1_Black = 0.012749</t>
+  </si>
+  <si>
+    <t>Color1_Brown = 0.011958</t>
+  </si>
+  <si>
+    <t>v1</t>
+  </si>
+  <si>
+    <t>v2 - did NOT get_dummy Breed_second</t>
+  </si>
+  <si>
+    <t># X features  = 278</t>
+  </si>
+  <si>
+    <t>Fixed_Intact = 0.265215</t>
+  </si>
+  <si>
+    <t>Fixed_Spayed = 0.096026</t>
+  </si>
+  <si>
+    <t>Fixed_Neutered = 0.071818</t>
+  </si>
+  <si>
+    <t>Mix = 0.046107</t>
+  </si>
+  <si>
+    <t>Sex_Male = 0.044345</t>
+  </si>
+  <si>
+    <t>Color2_White = 0.023359</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Baby = 0.018022</t>
+  </si>
+  <si>
+    <t>Color2_Tan = 0.014776</t>
+  </si>
+  <si>
+    <t>Color2_Black = 0.012750</t>
+  </si>
+  <si>
+    <t>Color1_Black = 0.012615</t>
+  </si>
+  <si>
+    <t>v3 - did NOT get_dummy Breed_second AND Color2</t>
+  </si>
+  <si>
+    <t># X features  = 244</t>
+  </si>
+  <si>
+    <t>Fixed_Intact = 0.319307</t>
+  </si>
+  <si>
+    <t>Fixed_Neutered = 0.109443</t>
+  </si>
+  <si>
+    <t>Fixed_Spayed = 0.086638</t>
+  </si>
+  <si>
+    <t>Mix = 0.047670</t>
+  </si>
+  <si>
+    <t>Sex_Male = 0.046585</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Baby = 0.018542</t>
+  </si>
+  <si>
+    <t>Color1_Black = 0.013635</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Adult = 0.013117</t>
+  </si>
+  <si>
+    <t>Color1_Tan = 0.012526</t>
+  </si>
+  <si>
+    <t>Color1_Brown = 0.012268</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>get_dummies vs OneHotEncoder?</t>
+  </si>
+  <si>
+    <t>dummy variable trap?</t>
+  </si>
+  <si>
+    <t>STILL USING GET_DUMMIES (not OneHotEncoder as mentioned in the label)</t>
+  </si>
+  <si>
+    <t>reducing the noise - taking top 20 colors?</t>
+  </si>
+  <si>
+    <t>v4 - did NOT get_dummy Breed_second AND Color2. Made Kelly changes(No Fix, Mix)</t>
+  </si>
+  <si>
+    <t># X features  = 410</t>
+  </si>
+  <si>
+    <t>Naïve Bayes</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Wow! # went down!</t>
+  </si>
+  <si>
+    <t>after taking Mix and Fixed</t>
+  </si>
+  <si>
+    <t>Sex_Male = 0.088696</t>
+  </si>
+  <si>
+    <t>Color1_Black = 0.033359</t>
+  </si>
+  <si>
+    <t>Color1_Tan = 0.032554</t>
+  </si>
+  <si>
+    <t>Color1_Brown = 0.030396</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Young = 0.025444</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Baby = 0.023535</t>
+  </si>
+  <si>
+    <t>Color1_White = 0.020884</t>
+  </si>
+  <si>
+    <t>Color1_Red = 0.019978</t>
+  </si>
+  <si>
+    <t>Pet_age_cat_Adult = 0.017655</t>
+  </si>
+  <si>
+    <t>Color1_Brown Brindle = 0.015820</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,8 +558,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,8 +584,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -416,11 +614,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -463,6 +698,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,33 +1026,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAF7CC1-A9BF-42AE-91D3-8A7A36BD33AD}">
-  <dimension ref="A1:AD34"/>
+  <dimension ref="A1:AD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.08984375" customWidth="1"/>
     <col min="2" max="2" width="33.453125" customWidth="1"/>
-    <col min="3" max="6" width="12.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="11.81640625" style="1" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.1796875" customWidth="1"/>
     <col min="10" max="10" width="18.08984375" customWidth="1"/>
     <col min="11" max="12" width="18.26953125" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" customWidth="1"/>
-    <col min="14" max="30" width="14.36328125" customWidth="1"/>
+    <col min="13" max="15" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="30" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14"/>
+      <c r="M2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
     </row>
     <row r="3" spans="1:30" s="7" customFormat="1" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -832,6 +1112,18 @@
       <c r="L3" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="M3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="4" spans="1:30" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
@@ -866,6 +1158,18 @@
       <c r="L4" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="M4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:30" s="7" customFormat="1" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
@@ -900,6 +1204,18 @@
       <c r="L5" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="M5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:30" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
@@ -928,6 +1244,18 @@
         <v>26</v>
       </c>
       <c r="L6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -954,6 +1282,18 @@
         <v>43</v>
       </c>
       <c r="L7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -975,6 +1315,18 @@
       </c>
       <c r="L8" s="6" t="s">
         <v>66</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:30" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -992,6 +1344,18 @@
         <v>78</v>
       </c>
       <c r="L9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P9" s="6" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1010,6 +1374,18 @@
       <c r="L10" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="M10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
@@ -1024,6 +1400,12 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
+      <c r="M11" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="21"/>
     </row>
     <row r="12" spans="1:30" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -1062,10 +1444,18 @@
       <c r="L12" s="11">
         <v>0.78080000000000005</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
+      <c r="M12" s="11">
+        <v>0.78029999999999999</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0.77990000000000004</v>
+      </c>
+      <c r="O12" s="11">
+        <v>0.78280000000000005</v>
+      </c>
+      <c r="P12" s="11">
+        <v>0.64690000000000003</v>
+      </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
@@ -1118,10 +1508,18 @@
       <c r="L13" s="15">
         <v>0.76900000000000002</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="M13" s="18">
+        <v>0.76749999999999996</v>
+      </c>
+      <c r="N13" s="18">
+        <v>0.76910000000000001</v>
+      </c>
+      <c r="O13" s="18">
+        <v>0.77749999999999997</v>
+      </c>
+      <c r="P13" s="18">
+        <v>0.61739999999999995</v>
+      </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
@@ -1150,10 +1548,10 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
@@ -1204,10 +1602,18 @@
       <c r="L15" s="11">
         <v>0.80679999999999996</v>
       </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
+      <c r="M15" s="11">
+        <v>0.80649999999999999</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0.80630000000000002</v>
+      </c>
+      <c r="O15" s="11">
+        <v>0.80620000000000003</v>
+      </c>
+      <c r="P15" s="11">
+        <v>0.66669999999999996</v>
+      </c>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
@@ -1258,10 +1664,18 @@
       <c r="L16" s="11">
         <v>0.80610000000000004</v>
       </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="M16" s="11">
+        <v>0.80579999999999996</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0.80610000000000004</v>
+      </c>
+      <c r="O16" s="11">
+        <v>0.8054</v>
+      </c>
+      <c r="P16" s="11">
+        <v>0.66690000000000005</v>
+      </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
@@ -1277,256 +1691,491 @@
       <c r="AC16" s="4"/>
       <c r="AD16" s="4"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G18" s="12" t="s">
+    <row r="17" spans="1:30" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11">
+        <v>0.36670000000000003</v>
+      </c>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+    </row>
+    <row r="18" spans="1:30" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F19" s="1" t="s">
+      <c r="M20" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G20" s="12" t="s">
+      <c r="M21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G21" s="12" t="s">
+      <c r="M22" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G23" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G22" s="12" t="s">
+      <c r="M23" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O23" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="L24" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G23" s="12" t="s">
+      <c r="M24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="L25" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G24" s="12" t="s">
+      <c r="M25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="P25" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G26" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G25" s="12" t="s">
+      <c r="M26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G27" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="L25" s="5" t="s">
+      <c r="L27" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G26" s="12" t="s">
+      <c r="M27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="O27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="P27" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G28" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H28" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K28" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="L28" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G27" s="12" t="s">
+      <c r="M28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="P28" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G29" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I29" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J29" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K29" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="L29" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G29" s="13" t="s">
+      <c r="M29" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G31" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K31" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L31" s="5" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="G30" s="13"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="M31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="17" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
+      <c r="P33" s="22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
+      <c r="P34" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
+      <c r="P35" s="23"/>
+    </row>
+    <row r="36" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>95</v>
       </c>
+      <c r="P36" s="23"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M11:P11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Gridsearch to RF model
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\GitlabContent\project-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498B5E7E-50A5-476D-A261-6AA3B782671D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EB16FD-54CB-47DA-AB90-1DD229A2D3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{1F03D750-29BA-4508-AE65-8D8AB8484A6A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="214">
   <si>
     <t>Random Forest (Train/Test split)</t>
   </si>
@@ -555,6 +555,126 @@
   </si>
   <si>
     <t>Top_colors_Tricolor       0.017633</t>
+  </si>
+  <si>
+    <t>May 22nd</t>
+  </si>
+  <si>
+    <t>ONE HOT ENCODING</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>Neural Network - 2 layer</t>
+  </si>
+  <si>
+    <t>Neural Network - 3 layer</t>
+  </si>
+  <si>
+    <t>Neural Network - 1 layer          Sequential model</t>
+  </si>
+  <si>
+    <t>model.compile(optimizer='adam',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              loss='categorical_crossentropy',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              metrics=['accuracy'])</t>
+  </si>
+  <si>
+    <t>sequential model()</t>
+  </si>
+  <si>
+    <t># Create model and add layers</t>
+  </si>
+  <si>
+    <t>model = Sequential()</t>
+  </si>
+  <si>
+    <t>model.add(Dense(units=100, activation='sigmoid', input_dim=397))</t>
+  </si>
+  <si>
+    <t>model.add(Dense(units=2, activation='softmax'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> # Compile and fit the model</t>
+  </si>
+  <si>
+    <t>model.compile(optimizer='sgd',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              loss='binary_crossentropy',</t>
+  </si>
+  <si>
+    <t>12006/12006 - 1s - loss: 0.6519 - accuracy: 0.6639</t>
+  </si>
+  <si>
+    <t>Normal Neural Network - Loss: 0.6519296946931477, Accuracy: 0.6639180183410645</t>
+  </si>
+  <si>
+    <t>model.add(Dense(units=400, activation='sigmoid', input_dim=397))</t>
+  </si>
+  <si>
+    <t>12006/12006 - 1s - loss: 0.6404 - accuracy: 0.6668</t>
+  </si>
+  <si>
+    <t>Normal Neural Network - Loss: 0.640447220533426, Accuracy: 0.666833221912384</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> model.fit(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    X_train,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    y_train,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    epochs=60,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    shuffle=True,</t>
+  </si>
+  <si>
+    <t>model.add(Dense(units=200, activation='relu', input_dim=397))</t>
+  </si>
+  <si>
+    <t>12006/12006 - 1s - loss: 0.7835 - accuracy: 0.6414</t>
+  </si>
+  <si>
+    <t>Normal Neural Network - Loss: 0.7834692467317449, Accuracy: 0.6414293050765991</t>
+  </si>
+  <si>
+    <t>model.add(Dense(units=100, activation='relu'))</t>
+  </si>
+  <si>
+    <t>12006/12006 - 1s - loss: 1.0630 - accuracy: 0.6551</t>
+  </si>
+  <si>
+    <t>Normal Neural Network - Loss: 1.0629517288579755, Accuracy: 0.6550891399383545</t>
+  </si>
+  <si>
+    <t>Took out Fixed</t>
+  </si>
+  <si>
+    <t>model.add(Dense(units=50, activation='relu'))</t>
+  </si>
+  <si>
+    <t>12006/12006 - 1s - loss: 1.1259 - accuracy: 0.6506</t>
+  </si>
+  <si>
+    <t>Normal Neural Network - Loss: 1.1258599197548786, Accuracy: 0.6505913734436035</t>
+  </si>
+  <si>
+    <t># Create model - 3 layers</t>
+  </si>
+  <si>
+    <t># Create model - 2 layers</t>
+  </si>
+  <si>
+    <t># Create model - 1 layer</t>
   </si>
 </sst>
 </file>
@@ -645,7 +765,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -668,35 +788,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -744,15 +840,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAAF7CC1-A9BF-42AE-91D3-8A7A36BD33AD}">
-  <dimension ref="A1:AD43"/>
+  <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M10" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20:Q29"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,55 +1181,103 @@
     <col min="2" max="2" width="33.453125" customWidth="1"/>
     <col min="3" max="3" width="11" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="6" width="11.81640625" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="27.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.1796875" customWidth="1"/>
     <col min="10" max="10" width="18.08984375" customWidth="1"/>
     <col min="11" max="12" width="18.26953125" customWidth="1"/>
     <col min="13" max="15" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="30" width="14.36328125" customWidth="1"/>
+    <col min="16" max="16" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="48" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="58.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="30" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="22" t="s">
         <v>156</v>
       </c>
+      <c r="R1" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="2" spans="1:30" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="M2" s="7" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
+      <c r="Q2" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="3" spans="1:30" s="7" customFormat="1" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
@@ -1171,6 +1321,18 @@
       <c r="Q3" s="6" t="s">
         <v>157</v>
       </c>
+      <c r="R3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="4" spans="1:30" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
@@ -1220,6 +1382,18 @@
       <c r="Q4" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="R4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:30" s="7" customFormat="1" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
@@ -1269,6 +1443,18 @@
       <c r="Q5" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="R5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:30" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
@@ -1312,6 +1498,18 @@
         <v>26</v>
       </c>
       <c r="Q6" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="U6" s="6" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1353,6 +1551,18 @@
         <v>43</v>
       </c>
       <c r="Q7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="U7" s="6" t="s">
         <v>159</v>
       </c>
     </row>
@@ -1388,6 +1598,18 @@
         <v>98</v>
       </c>
       <c r="Q8" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="U8" s="6" t="s">
         <v>160</v>
       </c>
     </row>
@@ -1421,6 +1643,18 @@
         <v>78</v>
       </c>
       <c r="Q9" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="U9" s="6" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1454,6 +1688,18 @@
       <c r="Q10" s="6" t="s">
         <v>81</v>
       </c>
+      <c r="R10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="U10" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
@@ -1468,13 +1714,25 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="21" t="s">
+      <c r="M11" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="23"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="T11" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="12" spans="1:30" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -1528,10 +1786,10 @@
       <c r="Q12" s="11">
         <v>0.64570000000000005</v>
       </c>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
-      <c r="U12" s="4"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
@@ -1594,10 +1852,10 @@
       <c r="Q13" s="18">
         <v>0.61429999999999996</v>
       </c>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
@@ -1626,10 +1884,10 @@
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
@@ -1690,10 +1948,10 @@
       <c r="Q15" s="11">
         <v>0.66890000000000005</v>
       </c>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
@@ -1754,10 +2012,10 @@
       <c r="Q16" s="11">
         <v>0.67</v>
       </c>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
@@ -1792,10 +2050,10 @@
       <c r="Q17" s="11">
         <v>0.36809999999999998</v>
       </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
@@ -1830,10 +2088,10 @@
       <c r="Q18" s="11">
         <v>0.66700000000000004</v>
       </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
@@ -1844,452 +2102,787 @@
       <c r="AC18" s="4"/>
       <c r="AD18" s="4"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="G20" s="12" t="s">
+    <row r="19" spans="1:30" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11">
+        <v>0.64070000000000005</v>
+      </c>
+      <c r="S19" s="11">
+        <v>0.63739999999999997</v>
+      </c>
+      <c r="T19" s="11">
+        <v>0.64380000000000004</v>
+      </c>
+      <c r="U19" s="11"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+    </row>
+    <row r="20" spans="1:30" ht="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="H21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="M20" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N21" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="O20" s="5" t="s">
+      <c r="O21" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="P20" s="5" t="s">
+      <c r="P21" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="Q20" s="5" t="s">
+      <c r="Q21" s="5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="F21" s="1" t="s">
+      <c r="R21" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="F22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G22" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K22" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="L22" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="M21" s="5" t="s">
+      <c r="M22" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N22" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="O21" s="5" t="s">
+      <c r="O22" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="P21" s="5" t="s">
+      <c r="P22" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="Q21" s="5" t="s">
+      <c r="Q22" s="5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="G22" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M22" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q22" s="5" t="s">
-        <v>166</v>
+      <c r="R22" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="V22" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="W22" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G23" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="V23" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="W23" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G24" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="V24" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="W24" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G25" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P25" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
+      </c>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="V25" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="W25" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G26" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P26" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>170</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G27" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P27" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
+      </c>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="V27" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="W27" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G28" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="V28" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="W28" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.35">
       <c r="G29" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="N29" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="O29" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="P29" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="V29" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="W29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G30" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="L29" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="M29" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N30" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="O29" s="5" t="s">
+      <c r="O30" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="P29" s="5" t="s">
+      <c r="P30" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="Q29" s="5" t="s">
+      <c r="Q30" s="5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="G30" s="13"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="V30" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="W30" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="G31" s="13" t="s">
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G32" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I31" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="K32" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="L31" s="5" t="s">
+      <c r="L32" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M31" s="5" t="s">
+      <c r="M32" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="N31" s="5" t="s">
+      <c r="N32" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="O31" s="5" t="s">
+      <c r="O32" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="P31" s="5" t="s">
+      <c r="P32" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="Q31" s="5" t="s">
+      <c r="Q32" s="5" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="G32" s="13"/>
-    </row>
-    <row r="33" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="17" t="s">
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="V32" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="W32" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="G33" s="13"/>
+      <c r="U33" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="V33" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="W33" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="P33" s="19" t="s">
+      <c r="P34" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="Q33" s="19" t="s">
+      <c r="Q34" s="19" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+    </row>
+    <row r="35" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="P34" s="20" t="s">
+      <c r="P35" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="Q34" s="20"/>
-    </row>
-    <row r="35" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="V35" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>94</v>
-      </c>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-    </row>
-    <row r="36" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="14" t="s">
-        <v>95</v>
       </c>
       <c r="P36" s="20"/>
       <c r="Q36" s="20"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
+      <c r="R36" s="20"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="V36" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="P37" s="20"/>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="20"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
+      <c r="U37" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="V37" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="U38" t="s">
+        <v>199</v>
+      </c>
+      <c r="V38" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="U39" t="s">
+        <v>200</v>
+      </c>
+      <c r="V39" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A41" s="17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="W42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="W43" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>139</v>
+      </c>
+      <c r="W44" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="W45" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="W46" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="W48" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W50" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W51" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W53" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="54" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W54" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W57" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="58" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W58" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="59" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W59" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W60" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W61" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="62" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W62" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="64" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W64" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W65" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W66" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W67" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W69" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="23:23" x14ac:dyDescent="0.35">
+      <c r="W70" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>